<commit_message>
Version 1.0.1-alpha.2. "Unknown" locality included in the list. Now it has a new list of localities to "uncheck" or remove from the table.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nahuel.delacruz\OneDrive - Sovos Compliance\Documents\UiPath\SUT_STS_VA_Filing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86D13FC-FB11-48F8-8F27-85F9CF3DF8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D136FE0B-D0E4-415A-BACD-60920D572B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="101">
   <si>
     <t>Name</t>
   </si>
@@ -264,9 +264,6 @@
     <t>ListLocalitiesWithNegativeNumbers</t>
   </si>
   <si>
-    <t>Unassigned</t>
-  </si>
-  <si>
     <t>Separate each locality with comma</t>
   </si>
   <si>
@@ -322,6 +319,15 @@
   </si>
   <si>
     <t>End of bot process</t>
+  </si>
+  <si>
+    <t>Unassigned,Unknown</t>
+  </si>
+  <si>
+    <t>ListLocalitiesToUncheck</t>
+  </si>
+  <si>
+    <t>Unknown</t>
   </si>
 </sst>
 </file>
@@ -699,8 +705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -838,28 +844,38 @@
         <v>78</v>
       </c>
       <c r="B16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" t="s">
         <v>79</v>
       </c>
-      <c r="C16" t="s">
-        <v>80</v>
-      </c>
     </row>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1837,7 +1853,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z991"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -2073,76 +2089,76 @@
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" t="s">
         <v>81</v>
-      </c>
-      <c r="B26" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27" t="s">
         <v>95</v>
-      </c>
-      <c r="B27" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28" t="s">
         <v>97</v>
-      </c>
-      <c r="B28" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" t="s">
         <v>92</v>
-      </c>
-      <c r="B29" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1">
       <c r="A33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1"/>

</xml_diff>